<commit_message>
some changes i made
</commit_message>
<xml_diff>
--- a/data/pandemic-legislation/american_rescue_plan.xlsx
+++ b/data/pandemic-legislation/american_rescue_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/Fiscal-Impact-Measure/data/pandemic-legislation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A497A2-AD43-484D-A928-FCAEECF979EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6056D716-614D-5F48-B697-5EFF3FD16988}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARP" sheetId="1" r:id="rId1"/>
@@ -1616,8 +1616,8 @@
   </sheetPr>
   <dimension ref="A1:BA989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1637,7 +1637,8 @@
     <col min="17" max="17" width="13" customWidth="1"/>
     <col min="18" max="19" width="29" customWidth="1"/>
     <col min="20" max="23" width="34.5" customWidth="1"/>
-    <col min="24" max="25" width="18.5" customWidth="1"/>
+    <col min="24" max="24" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5" customWidth="1"/>
     <col min="26" max="27" width="25.83203125" customWidth="1"/>
     <col min="28" max="28" width="28.6640625" customWidth="1"/>
     <col min="29" max="30" width="26.5" customWidth="1"/>
@@ -4353,7 +4354,10 @@
       <c r="Z27" s="36"/>
       <c r="AA27" s="36"/>
       <c r="AC27" s="40"/>
-      <c r="AE27" s="14"/>
+      <c r="AE27" s="14">
+        <f>334+28</f>
+        <v>362</v>
+      </c>
       <c r="AF27" s="52"/>
       <c r="AL27" s="31"/>
       <c r="AM27" s="25"/>
@@ -4382,7 +4386,10 @@
       <c r="Z28" s="36"/>
       <c r="AA28" s="36"/>
       <c r="AC28" s="40"/>
-      <c r="AE28" s="14"/>
+      <c r="AE28" s="14">
+        <f>AE27*4</f>
+        <v>1448</v>
+      </c>
       <c r="AF28" s="52"/>
       <c r="AL28" s="31"/>
       <c r="AM28" s="25"/>
@@ -4410,7 +4417,9 @@
       <c r="Z29" s="36"/>
       <c r="AA29" s="36"/>
       <c r="AC29" s="40"/>
-      <c r="AE29" s="14"/>
+      <c r="AE29" s="14">
+        <v>36465.42</v>
+      </c>
       <c r="AF29" s="52"/>
       <c r="AL29" s="31"/>
       <c r="AM29" s="25"/>

</xml_diff>